<commit_message>
finalizada automatizacion caso altero y caso exitoso
</commit_message>
<xml_diff>
--- a/src/test/resources/DataDriven/dataDrivenEriBank.xlsx
+++ b/src/test/resources/DataDriven/dataDrivenEriBank.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>monto</t>
+  </si>
+  <si>
+    <t>compan2</t>
+  </si>
+  <si>
+    <t>company2</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -475,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EW2"/>
+  <dimension ref="A1:EW3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.58203125" defaultRowHeight="19.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -547,6 +559,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:153" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>